<commit_message>
Documentation of cloud scores improved
</commit_message>
<xml_diff>
--- a/doc/Properties table.xlsx
+++ b/doc/Properties table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="14220"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="IAF" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="19">
   <si>
     <t>b1 original</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Characteristics of IAF cloud decompositions</t>
+  </si>
+  <si>
+    <t>o3 cloud score</t>
+  </si>
+  <si>
+    <t>o1, o3 and luck</t>
+  </si>
+  <si>
+    <t>Characteristics of datum cloud decompositions</t>
+  </si>
+  <si>
+    <t>b3 datum scores</t>
   </si>
 </sst>
 </file>
@@ -101,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +129,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -222,9 +240,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -235,9 +250,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -246,6 +258,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -526,324 +548,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G5" sqref="G5:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G1" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+      <c r="G6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="23"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="21"/>
+      <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="21"/>
+      <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
+      <c r="G8" s="21"/>
+      <c r="H8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="21"/>
+      <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="9"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="9"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6" t="s">
+      <c r="E11" s="8"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="11"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
+      <c r="G14" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="23"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
+      <c r="G15" s="21"/>
+      <c r="H15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="23"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6" t="s">
+      <c r="G17" s="21"/>
+      <c r="H17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="9"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="9"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22"/>
+      <c r="B20" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6" t="s">
+      <c r="C20" s="13"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="14"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="16"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A22:A28"/>
+    <mergeCell ref="A6:A12"/>
     <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="G6:G12"/>
+    <mergeCell ref="G14:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -864,7 +865,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>14</v>
       </c>
     </row>
@@ -883,285 +884,285 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="19"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="21"/>
+      <c r="B15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="21"/>
+      <c r="B17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="21"/>
+      <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="21"/>
+      <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="21"/>
+      <c r="B20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="21"/>
+      <c r="B23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="21"/>
+      <c r="B24" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="21"/>
+      <c r="B25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6" t="s">
+      <c r="A26" s="21"/>
+      <c r="B26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="21"/>
+      <c r="B27" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6" t="s">
+      <c r="A28" s="21"/>
+      <c r="B28" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="19"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17"/>
     </row>
     <row r="29" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="19"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6" t="s">
+      <c r="A31" s="21"/>
+      <c r="B31" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="21"/>
+      <c r="B32" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="19"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="17"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6" t="s">
+      <c r="A33" s="21"/>
+      <c r="B33" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="19"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6" t="s">
+      <c r="A34" s="21"/>
+      <c r="B34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="19"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="17"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="21"/>
+      <c r="B35" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="19"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="17"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="14" t="s">
+      <c r="A36" s="22"/>
+      <c r="B36" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>